<commit_message>
add filter bee cells in lte
</commit_message>
<xml_diff>
--- a/tests/reports/network-vs-atoll.xlsx
+++ b/tests/reports/network-vs-atoll.xlsx
@@ -537,7 +537,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>lcell1</t>
+          <t>L2100cell</t>
         </is>
       </c>
     </row>
@@ -549,12 +549,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>lsite2</t>
+          <t>ERBS_555</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>lcell2</t>
+          <t>L1800</t>
         </is>
       </c>
     </row>
@@ -566,12 +566,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>lsite3</t>
+          <t>ERBS_777</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>lcell3</t>
+          <t>cell3</t>
         </is>
       </c>
     </row>

</xml_diff>